<commit_message>
Python IoT AV1 02maio2023
</commit_message>
<xml_diff>
--- a/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
+++ b/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\24 WydenArea1AplicacaoCloudIndustria40Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\24 WydenArea1AplicacaoCloudIndustria40Python\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9F625D-2058-454B-8DB1-E5502A9911DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAAB064-5CD3-4C54-8000-73C4CA7E9E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37207522-E8FF-4681-8F81-32F57A53DE4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Equipe</t>
   </si>
@@ -80,18 +80,9 @@
     <t>Franklin Souza</t>
   </si>
   <si>
-    <t>Web; Github</t>
-  </si>
-  <si>
-    <t>Web; Github (não); Leitor de Scripts</t>
-  </si>
-  <si>
     <t>Angelo do Nascimento</t>
   </si>
   <si>
-    <t>Github; Web; Cadastro de Fornecedores</t>
-  </si>
-  <si>
     <t>postou atividade de cloud computer (url)</t>
   </si>
   <si>
@@ -110,18 +101,9 @@
     <t>Matheus Matos</t>
   </si>
   <si>
-    <t>Github; API para integrar produtos Shp</t>
-  </si>
-  <si>
     <t>Adrielle Santana</t>
   </si>
   <si>
-    <t>Github; Projeto Arduino</t>
-  </si>
-  <si>
-    <t>Github; Universo Colaborativo</t>
-  </si>
-  <si>
     <t>Raudiney Andrade</t>
   </si>
   <si>
@@ -134,9 +116,6 @@
     <t>Vinicius</t>
   </si>
   <si>
-    <t>MKV; BI Cotações do Ibovespa;</t>
-  </si>
-  <si>
     <t>Faltou ???</t>
   </si>
   <si>
@@ -149,13 +128,40 @@
     <t>Klaus Erick Maciel</t>
   </si>
   <si>
-    <t>Github; enviar email; Não Equipe de João Pamponet Projeto Arduino</t>
-  </si>
-  <si>
     <t>***</t>
   </si>
   <si>
     <t>Notas: AV1 - Projetos Python IoT - 01/05/2023</t>
+  </si>
+  <si>
+    <t>Thauan</t>
+  </si>
+  <si>
+    <t>Luiz Junior</t>
+  </si>
+  <si>
+    <t>Parabéns Klaus, envio de e-mail; Github; enviar email; Não Equipe de João Pamponet Projeto Arduino</t>
+  </si>
+  <si>
+    <t>Web; Github; Lista de Tarefas; Não edita; não consulta; https://projetowebpython.onrender.com/</t>
+  </si>
+  <si>
+    <t>Web; Github (não); Leitor de Scripts; não remove; não guarda no BD; https://filgueiras7-leitorscript-app-x4nmz3.streamlit.app/</t>
+  </si>
+  <si>
+    <t>Github; Web; Cadastro de Fornecedores; informar o atributo de busca; validar atributos, ex. e-mail; https://projetofullstackpython-production.up.railway.app/</t>
+  </si>
+  <si>
+    <t>Github; API para integrar produtos Shp; Time Solidário (ensino API/GIT). https://github.com/EvertonMutti/API_Shopping</t>
+  </si>
+  <si>
+    <t>Github; Projeto Arduino; https://github.com/JV1T0R/Arduino-project; Projeto não rodando</t>
+  </si>
+  <si>
+    <t>WEB(não); Github(Não); Vídeo MKV; BI Cotações do Ibovespa; faltou a analise dos dados; quando investir; quanto investir; consultoria financeira.</t>
+  </si>
+  <si>
+    <t>Github não; Universo Colaborativo; VSCode; Posts (consulta; delete; alteração); js dinâmico; sem API</t>
   </si>
 </sst>
 </file>
@@ -614,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AED4F9D-46A6-4463-AA32-0C4C94548B61}">
-  <dimension ref="B1:H53"/>
+  <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +634,7 @@
   <sheetData>
     <row r="1" spans="3:8" s="11" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D1" s="12" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
@@ -658,9 +664,14 @@
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0</v>
+      </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
@@ -675,211 +686,265 @@
       <c r="D9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="14">
+        <v>7</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
       <c r="G9" s="14"/>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="16"/>
-      <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="16"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
       <c r="G11" s="14"/>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" t="s">
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="2"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>7.8</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>4</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="3" t="s">
-        <v>23</v>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="D21" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>5</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="14"/>
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H22" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25">
         <v>7</v>
       </c>
-      <c r="H24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>6</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D28" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="7" t="s">
-        <v>36</v>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32">
+      <c r="D32" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36">
         <v>6</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <v>7</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D35" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39">
-        <v>8</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" t="s">
-        <v>19</v>
+      <c r="F40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
       <c r="D41" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D49" s="13"/>
-    </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="H53" s="15"/>
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D46" s="13"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Python IoT AV1 03maio2023
</commit_message>
<xml_diff>
--- a/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
+++ b/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\24 WydenArea1AplicacaoCloudIndustria40Python\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAAB064-5CD3-4C54-8000-73C4CA7E9E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1B80C0-87E4-4820-9790-A759C0A25B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37207522-E8FF-4681-8F81-32F57A53DE4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Equipe</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Angelo do Nascimento</t>
   </si>
   <si>
-    <t>postou atividade de cloud computer (url)</t>
-  </si>
-  <si>
     <t>IA; http://ec2-18-231-186-141.sa-east-1.compute.amazonaws.com/</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Rafael</t>
   </si>
   <si>
-    <t>Vinicius</t>
-  </si>
-  <si>
     <t>Faltou ???</t>
   </si>
   <si>
@@ -137,15 +131,9 @@
     <t>Thauan</t>
   </si>
   <si>
-    <t>Luiz Junior</t>
-  </si>
-  <si>
     <t>Parabéns Klaus, envio de e-mail; Github; enviar email; Não Equipe de João Pamponet Projeto Arduino</t>
   </si>
   <si>
-    <t>Web; Github; Lista de Tarefas; Não edita; não consulta; https://projetowebpython.onrender.com/</t>
-  </si>
-  <si>
     <t>Web; Github (não); Leitor de Scripts; não remove; não guarda no BD; https://filgueiras7-leitorscript-app-x4nmz3.streamlit.app/</t>
   </si>
   <si>
@@ -162,13 +150,34 @@
   </si>
   <si>
     <t>Github não; Universo Colaborativo; VSCode; Posts (consulta; delete; alteração); js dinâmico; sem API</t>
+  </si>
+  <si>
+    <t>Fez sozinho. Web; Github; Lista de Tarefas; Não edita; não consulta; https://projetowebpython.onrender.com/</t>
+  </si>
+  <si>
+    <t>sozinho</t>
+  </si>
+  <si>
+    <t>sozinha</t>
+  </si>
+  <si>
+    <t>Vinicius Jesus Santos</t>
+  </si>
+  <si>
+    <t>Luiz Carlos Junior</t>
+  </si>
+  <si>
+    <t>POST http://127.0.0.1:5000/post net::ERR_CONNECTION_REFUSED; Cannot GET /post</t>
+  </si>
+  <si>
+    <t>postou atividade de cloud computer (url); instalei as dependências pip cors; pis flask; pip datetime; não validou e-mail; ESTADO inválido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,8 +220,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +287,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -305,6 +328,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -620,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AED4F9D-46A6-4463-AA32-0C4C94548B61}">
-  <dimension ref="B1:H50"/>
+  <dimension ref="B1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,12 +657,12 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" s="11" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="11" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D1" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -657,7 +682,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="C5">
         <v>1</v>
       </c>
@@ -671,159 +699,174 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="14">
+        <v>7</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="14">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
       </c>
       <c r="F9" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
-        <v>9</v>
-      </c>
-      <c r="F11" s="14">
-        <v>0</v>
-      </c>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="2"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>4</v>
-      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>7.8</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16">
-        <v>7.8</v>
+        <v>19</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="D19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20">
+      <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="14">
-        <v>0</v>
-      </c>
       <c r="H20" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D21" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23">
         <v>7</v>
       </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <v>6</v>
-      </c>
       <c r="D25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="F25">
         <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -832,119 +875,106 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="7" t="s">
+      <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="F27">
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29">
-        <v>6</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" t="s">
-        <v>28</v>
-      </c>
       <c r="H29" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <v>7</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="H31" t="s">
-        <v>40</v>
+      <c r="D31" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D32" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D33" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D34" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36">
-        <v>8</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36">
-        <v>6</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="H36" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
       <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>2</v>
       </c>
-      <c r="D40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F40">
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s">
-        <v>33</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="13"/>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H50" s="15"/>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D44" s="13"/>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Cloud Computer AV1 04maio2023
</commit_message>
<xml_diff>
--- a/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
+++ b/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\24 WydenArea1AplicacaoCloudIndustria40Python\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1B80C0-87E4-4820-9790-A759C0A25B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA7125B-252D-433B-9E33-3960790BA878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37207522-E8FF-4681-8F81-32F57A53DE4E}"/>
   </bookViews>
@@ -170,7 +170,7 @@
     <t>POST http://127.0.0.1:5000/post net::ERR_CONNECTION_REFUSED; Cannot GET /post</t>
   </si>
   <si>
-    <t>postou atividade de cloud computer (url); instalei as dependências pip cors; pis flask; pip datetime; não validou e-mail; ESTADO inválido</t>
+    <t>postou atividade de cloud computer (url); instalei as dependências pip cors; pis flask; pip datetime; não validou e-mail; ESTADO inválido SEM bd</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Aula 08 Cloud IoT Python Indústria 4.0 e Outros 09maio2023
</commit_message>
<xml_diff>
--- a/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
+++ b/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\24 WydenArea1AplicacaoCloudIndustria40Python\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA7125B-252D-433B-9E33-3960790BA878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E6FDC3-613A-48EF-9E82-292258A4B712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37207522-E8FF-4681-8F81-32F57A53DE4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Equipe</t>
   </si>
@@ -104,15 +104,6 @@
     <t>Raudiney Andrade</t>
   </si>
   <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Rafael</t>
-  </si>
-  <si>
-    <t>Faltou ???</t>
-  </si>
-  <si>
     <t>Caike Rocha</t>
   </si>
   <si>
@@ -171,13 +162,28 @@
   </si>
   <si>
     <t>postou atividade de cloud computer (url); instalei as dependências pip cors; pis flask; pip datetime; não validou e-mail; ESTADO inválido SEM bd</t>
+  </si>
+  <si>
+    <t>Kerven</t>
+  </si>
+  <si>
+    <t>Só Quiz</t>
+  </si>
+  <si>
+    <t>Deividy Cardoso</t>
+  </si>
+  <si>
+    <t>Raphael Braga</t>
+  </si>
+  <si>
+    <t>Só Quiz; Desistiu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +234,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +307,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -330,6 +350,9 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -645,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AED4F9D-46A6-4463-AA32-0C4C94548B61}">
-  <dimension ref="B1:H48"/>
+  <dimension ref="B1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +682,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="11" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D1" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -684,7 +707,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -699,12 +722,12 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -720,7 +743,7 @@
       </c>
       <c r="G7" s="14"/>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -742,239 +765,234 @@
       </c>
       <c r="G9" s="14"/>
       <c r="H9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>7.8</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>4</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14">
-        <v>7.8</v>
+        <v>19</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="D17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="14">
-        <v>0</v>
-      </c>
       <c r="H18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21">
         <v>7</v>
       </c>
-      <c r="H20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="18"/>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <v>6</v>
-      </c>
       <c r="D23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="H23" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D24" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25">
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" t="s">
-        <v>26</v>
-      </c>
       <c r="H27" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <v>7</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29">
-        <v>7</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>36</v>
+      <c r="D29" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D30" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D31" s="9" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="9" t="s">
-        <v>41</v>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>6.5</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <v>8</v>
-      </c>
       <c r="D34" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38">
         <v>10</v>
       </c>
-      <c r="E34">
-        <v>6</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>30</v>
+      <c r="D38" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D44" s="13"/>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H48" s="15"/>
+      <c r="H38" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D42" s="13"/>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Cloud IoT Python ajustes 20Jun2023
</commit_message>
<xml_diff>
--- a/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
+++ b/03 Assessments/notas AV1 Python IoT 02Maio2023 yduqs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\24 WydenArea1AplicacaoCloudIndustria40Python\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E6FDC3-613A-48EF-9E82-292258A4B712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFE2F44-EEFC-4210-AFE8-4CB810B99B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37207522-E8FF-4681-8F81-32F57A53DE4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Equipe</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Vinicius Scandura</t>
   </si>
   <si>
-    <t>AV1</t>
-  </si>
-  <si>
     <t>Ariel Araujo</t>
   </si>
   <si>
@@ -167,23 +164,29 @@
     <t>Kerven</t>
   </si>
   <si>
-    <t>Só Quiz</t>
-  </si>
-  <si>
     <t>Deividy Cardoso</t>
   </si>
   <si>
     <t>Raphael Braga</t>
   </si>
   <si>
-    <t>Só Quiz; Desistiu</t>
+    <t>AV1/AV2</t>
+  </si>
+  <si>
+    <t>+1 apresentação seminário Microcontroladores</t>
+  </si>
+  <si>
+    <t>Só Quiz; Desistiu; TRANCOU</t>
+  </si>
+  <si>
+    <t>Só Quiz; Desistiu ???</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +241,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -353,6 +364,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -668,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AED4F9D-46A6-4463-AA32-0C4C94548B61}">
-  <dimension ref="B1:H46"/>
+  <dimension ref="B1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +695,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="11" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D1" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -693,13 +706,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
         <v>3</v>
@@ -707,13 +720,13 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -721,13 +734,17 @@
       <c r="F5" s="14">
         <v>0</v>
       </c>
+      <c r="G5">
+        <f>E5+F5</f>
+        <v>7</v>
+      </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -741,21 +758,23 @@
       <c r="F7" s="14">
         <v>1</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7">
+        <f t="shared" ref="G6:G38" si="0">E7+F7</f>
+        <v>8</v>
+      </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9">
         <v>9</v>
@@ -763,9 +782,12 @@
       <c r="F9" s="14">
         <v>0</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -773,18 +795,17 @@
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12">
         <v>7.8</v>
@@ -792,24 +813,44 @@
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000007</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>7.8</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="E14">
+        <v>7.8</v>
       </c>
       <c r="F14">
         <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C16">
@@ -824,40 +865,72 @@
       <c r="F16" s="14">
         <v>0</v>
       </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="H16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="H17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="H19" s="18"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21">
         <v>7</v>
@@ -865,48 +938,107 @@
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H21" s="23">
+        <v>9</v>
+      </c>
+      <c r="I21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H22" s="23">
+        <v>9</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="7" t="s">
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H23" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="7" t="s">
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H24" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>25</v>
       </c>
       <c r="C25">
         <v>6</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H25" s="23">
+        <v>9</v>
+      </c>
+      <c r="I25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>7</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27">
         <v>7</v>
@@ -914,31 +1046,65 @@
       <c r="F27">
         <v>1</v>
       </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="H27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D28" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D29" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D30" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>8</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32">
         <v>6.5</v>
@@ -946,18 +1112,42 @@
       <c r="F32">
         <v>0</v>
       </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D33" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>6.5</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="E34">
+        <v>6.5</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
       </c>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
@@ -965,13 +1155,20 @@
         <v>9</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
-      <c r="H36" t="s">
-        <v>43</v>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
@@ -979,9 +1176,16 @@
         <v>10</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
       </c>
       <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H38" s="21" t="s">

</xml_diff>